<commit_message>
adjust config file for input
</commit_message>
<xml_diff>
--- a/config/config_pub_files.xlsx
+++ b/config/config_pub_files.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hettnekm1/OAscript/OAmonitoring/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitoring/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E46F2A-2CCD-4943-B1AB-8425811D7A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA431FE2-EAB7-3646-A5DE-75BD6000F0CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="540" windowWidth="28040" windowHeight="15940" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
@@ -31,51 +31,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
-  <si>
-    <t>File 1</t>
-  </si>
-  <si>
-    <t>File 2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>ISSN</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>scopus_social_evol_2018.csv</t>
+  </si>
+  <si>
+    <t>wos_digital_humanities_2018.tsv</t>
+  </si>
+  <si>
+    <t>EID</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>Internal unique identifier</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>File_info</t>
   </si>
   <si>
     <t>File</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>ISSN</t>
-  </si>
-  <si>
-    <t>DOI</t>
-  </si>
-  <si>
-    <t>scopus_social_evol_2018.csv</t>
-  </si>
-  <si>
-    <t>wos_digital_humanities_2018.tsv</t>
-  </si>
-  <si>
-    <t>EID</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>UT</t>
-  </si>
-  <si>
-    <t>DI</t>
-  </si>
-  <si>
-    <t>SN</t>
-  </si>
-  <si>
-    <t>Internal unique identifier</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -430,7 +427,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,68 +439,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made an extension booboo
</commit_message>
<xml_diff>
--- a/config/config_pub_files.xlsx
+++ b/config/config_pub_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitoring/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA431FE2-EAB7-3646-A5DE-75BD6000F0CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7270D8-986F-F544-AD98-0EBBE5556F65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="540" windowWidth="28040" windowHeight="15940" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Title</t>
   </si>
@@ -42,12 +42,6 @@
     <t>DOI</t>
   </si>
   <si>
-    <t>scopus_social_evol_2018.csv</t>
-  </si>
-  <si>
-    <t>wos_digital_humanities_2018.tsv</t>
-  </si>
-  <si>
     <t>EID</t>
   </si>
   <si>
@@ -73,6 +67,18 @@
   </si>
   <si>
     <t>File</t>
+  </si>
+  <si>
+    <t>Organization unit</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>mockdata_dighum_2018.csv</t>
+  </si>
+  <si>
+    <t>mockdata_niche_2018.tsv</t>
   </si>
 </sst>
 </file>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD2166A-EC47-ED44-87CF-C15299393BC9}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,40 +443,43 @@
     <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -478,10 +487,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -489,10 +501,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -500,7 +512,18 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
troubleshooting with config file
</commit_message>
<xml_diff>
--- a/config/config_pub_files.xlsx
+++ b/config/config_pub_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitoring/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7270D8-986F-F544-AD98-0EBBE5556F65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2820A84-0807-3540-90E7-E8355FBF3AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="540" windowWidth="28040" windowHeight="15940" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Title</t>
   </si>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD2166A-EC47-ED44-87CF-C15299393BC9}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,7 +443,7 @@
     <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -453,11 +453,8 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -468,7 +465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -479,7 +476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -489,11 +486,8 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -504,7 +498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -515,7 +509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
adjusted layout on configuration for files
</commit_message>
<xml_diff>
--- a/config/config_pub_files.xlsx
+++ b/config/config_pub_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitoring/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2820A84-0807-3540-90E7-E8355FBF3AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AA8BE8-3ACB-7C4A-8422-BBF62F4A7F06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="540" windowWidth="28040" windowHeight="15940" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -93,16 +93,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,12 +139,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,95 +477,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD2166A-EC47-ED44-87CF-C15299393BC9}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
config file adjusted to fit changed demands
</commit_message>
<xml_diff>
--- a/config/config_pub_files.xlsx
+++ b/config/config_pub_files.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitoring/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/OAreport/2019/OAmonitoring_UU2019_WoS/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AA8BE8-3ACB-7C4A-8422-BBF62F4A7F06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52643CC-BB67-034C-A485-D68E3AEC82D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="540" windowWidth="28040" windowHeight="15940" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
+    <workbookView xWindow="760" yWindow="540" windowWidth="13080" windowHeight="17260" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>ISSN</t>
   </si>
@@ -45,9 +42,6 @@
     <t>EID</t>
   </si>
   <si>
-    <t>TI</t>
-  </si>
-  <si>
     <t>UT</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>File</t>
   </si>
   <si>
-    <t>Organization unit</t>
-  </si>
-  <si>
     <t>subject</t>
   </si>
   <si>
@@ -79,6 +70,33 @@
   </si>
   <si>
     <t>mockdata_niche_2018.tsv</t>
+  </si>
+  <si>
+    <t>Other columns to include</t>
+  </si>
+  <si>
+    <t>EI</t>
+  </si>
+  <si>
+    <t>Format (tsv, csv, xls, or xlsx)</t>
+  </si>
+  <si>
+    <t>EISSN (electronic ISSN)</t>
+  </si>
+  <si>
+    <t>tsv</t>
+  </si>
+  <si>
+    <t>Departments and/or faculties</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>TI, SO, PU, SC</t>
+  </si>
+  <si>
+    <t>Title, Source title, Publisher</t>
   </si>
 </sst>
 </file>
@@ -158,11 +176,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD2166A-EC47-ED44-87CF-C15299393BC9}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,13 +512,13 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -508,13 +528,13 @@
     </row>
     <row r="2" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -524,13 +544,13 @@
     </row>
     <row r="3" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -540,13 +560,13 @@
     </row>
     <row r="4" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -556,13 +576,13 @@
     </row>
     <row r="5" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -572,13 +592,11 @@
     </row>
     <row r="6" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -588,13 +606,13 @@
     </row>
     <row r="7" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -602,8 +620,37 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed nonexistent column from selection
</commit_message>
<xml_diff>
--- a/config/config_pub_files.xlsx
+++ b/config/config_pub_files.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/OAreport/2019/OAmonitoring_UU2019_WoS/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitoring/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52643CC-BB67-034C-A485-D68E3AEC82D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905B082F-F5B4-3946-8F81-A278CED58395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="540" windowWidth="13080" windowHeight="17260" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
@@ -93,10 +93,10 @@
     <t>csv</t>
   </si>
   <si>
-    <t>TI, SO, PU, SC</t>
-  </si>
-  <si>
     <t>Title, Source title, Publisher</t>
+  </si>
+  <si>
+    <t>SO, PU, SC</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,10 +641,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>

</xml_diff>

<commit_message>
load all columns in example
</commit_message>
<xml_diff>
--- a/config/config_pub_files.xlsx
+++ b/config/config_pub_files.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barbaramaria/surfdrive/Programming/OAmonitoring/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905B082F-F5B4-3946-8F81-A278CED58395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A0AFC3-9A93-FE48-89DD-3F980182D3FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="540" windowWidth="13080" windowHeight="17260" xr2:uid="{EC4569DB-D389-4344-A1CE-1A1B2B7F57C3}"/>
   </bookViews>
@@ -93,10 +93,10 @@
     <t>csv</t>
   </si>
   <si>
-    <t>Title, Source title, Publisher</t>
-  </si>
-  <si>
     <t>SO, PU, SC</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,10 +641,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>

</xml_diff>